<commit_message>
add: agregué una planilla con las fechas del cronograma
</commit_message>
<xml_diff>
--- a/Minutas.xlsx
+++ b/Minutas.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Minutas" sheetId="1" r:id="rId1"/>
+    <sheet name="Fechas estimativas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Fecha</t>
   </si>
@@ -58,12 +59,72 @@
       <t xml:space="preserve"> para el tracking, acuerdo de pasos iniciales, creacion de repositorio. </t>
     </r>
   </si>
+  <si>
+    <t>Espera firmas protocolo</t>
+  </si>
+  <si>
+    <t>No empezamos con la primera etapa ya que estuvimos esperando documentacion.</t>
+  </si>
+  <si>
+    <t>Etapa</t>
+  </si>
+  <si>
+    <t>Tarea</t>
+  </si>
+  <si>
+    <t>Análisis e Investigación de herramientas y tecnologias a utilizar</t>
+  </si>
+  <si>
+    <t>Relevamiento de requerimientos</t>
+  </si>
+  <si>
+    <t>Diseño de arquitectura</t>
+  </si>
+  <si>
+    <t>Modelo deteccion de entidades: Recopilacion y etiquetado de datos</t>
+  </si>
+  <si>
+    <t>Implementacion de modelo de deteccion de entidades</t>
+  </si>
+  <si>
+    <t>Testeo y Entrenamiento de modelo de entidades</t>
+  </si>
+  <si>
+    <t>Validación del modelo con datos reales</t>
+  </si>
+  <si>
+    <t>Modelo violencia de género: Recopilacion y etiquetado de datos</t>
+  </si>
+  <si>
+    <t>Implementacion de modelo de deteccion de violencia de género</t>
+  </si>
+  <si>
+    <t>Testeo y entrenamiento de modelo de deteccion de violencia de género</t>
+  </si>
+  <si>
+    <t>Implementacion de servidor backend</t>
+  </si>
+  <si>
+    <t>Implementacion de interfaz web: Carga de datos y uso de modelos.</t>
+  </si>
+  <si>
+    <t>Implementacion de interfaz web: Visualizacion de resultados.</t>
+  </si>
+  <si>
+    <t>Fecha inicio</t>
+  </si>
+  <si>
+    <t>Fecha Fin Etapa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,16 +140,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -96,20 +202,187 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -120,7 +393,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
@@ -128,6 +401,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -414,53 +692,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D27"/>
+  <dimension ref="B3:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19" style="1" customWidth="1"/>
-    <col min="4" max="4" width="47" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+    <row r="4" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>44858</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
         <v>44866</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -479,4 +768,206 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="57.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="16">
+        <v>44858</v>
+      </c>
+      <c r="E3" s="18">
+        <v>44914</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="16">
+        <v>44879</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6"/>
+      <c r="C5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="16">
+        <v>44900</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="16">
+        <v>44914</v>
+      </c>
+      <c r="E6" s="19">
+        <v>44991</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="16">
+        <v>44942</v>
+      </c>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="16">
+        <v>44970</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="7"/>
+      <c r="C9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="16">
+        <v>44984</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="16">
+        <v>44991</v>
+      </c>
+      <c r="E10" s="20">
+        <v>45068</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="16">
+        <v>45019</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="16">
+        <v>45047</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="8"/>
+      <c r="C13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="16">
+        <v>45061</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="9">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="16">
+        <v>45068</v>
+      </c>
+      <c r="E14" s="21">
+        <v>44773</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="16">
+        <v>45089</v>
+      </c>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
+      <c r="C16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="16">
+        <v>45103</v>
+      </c>
+      <c r="E16" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E14:E16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add: reunion a minutas
</commit_message>
<xml_diff>
--- a/Minutas.xlsx
+++ b/Minutas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Minutas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Fecha</t>
   </si>
@@ -116,13 +116,19 @@
   <si>
     <t>Fecha Fin Etapa</t>
   </si>
+  <si>
+    <t>Reunion Requerimientos</t>
+  </si>
+  <si>
+    <t>Repasamos el documento de requerimientos y continuamos con su elaboracion. Definimos dudas a resolver con los demandantes.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -338,6 +344,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -350,28 +378,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -694,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +745,17 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>44899</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="7" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -774,14 +790,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="57.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="10" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -793,21 +809,21 @@
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="12">
         <v>44858</v>
       </c>
       <c r="E3" s="18">
@@ -815,33 +831,33 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="12">
         <v>44879</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6"/>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="12">
         <v>44900</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="7">
+      <c r="B6" s="15">
         <v>2</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="12">
         <v>44914</v>
       </c>
       <c r="E6" s="19">
@@ -849,43 +865,43 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="12">
         <v>44942</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="12">
         <v>44970</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="7"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="12">
         <v>44984</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="8">
+      <c r="B10" s="16">
         <v>3</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="12">
         <v>44991</v>
       </c>
       <c r="E10" s="20">
@@ -893,43 +909,43 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="12">
         <v>45019</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="12">
         <v>45047</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="8"/>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="12">
         <v>45061</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="16"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="9">
+      <c r="B14" s="17">
         <v>4</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="12">
         <v>45068</v>
       </c>
       <c r="E14" s="21">
@@ -937,24 +953,24 @@
       </c>
     </row>
     <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="12">
         <v>45089</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="9"/>
-      <c r="C16" s="12" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="12">
         <v>45103</v>
       </c>
-      <c r="E16" s="9"/>
+      <c r="E16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
update: minutas y backup tiempo
</commit_message>
<xml_diff>
--- a/Minutas.xlsx
+++ b/Minutas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Minutas" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>Fecha</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Horas estimadas</t>
   </si>
   <si>
-    <t>DISEÑO DE INTERFACES</t>
-  </si>
-  <si>
     <t>Reunion: Casos de uso</t>
   </si>
   <si>
@@ -155,6 +152,51 @@
   </si>
   <si>
     <t>Horas reales</t>
+  </si>
+  <si>
+    <t>Fecha fin Real</t>
+  </si>
+  <si>
+    <t>DISEÑO DE INTERFACES (tarea extra)</t>
+  </si>
+  <si>
+    <t>Reunion interfaces</t>
+  </si>
+  <si>
+    <t>Definimos las pantallas a diseñar y presentamos la aplicacion figma.</t>
+  </si>
+  <si>
+    <t>EMPIEZA ETAPA 2? 1.5?</t>
+  </si>
+  <si>
+    <t>Empezamos el diseño de interfaces</t>
+  </si>
+  <si>
+    <t>Reunion Diseño</t>
+  </si>
+  <si>
+    <t>Nos reunimos de forma presencial para continuar el diseño de las interfaces.</t>
+  </si>
+  <si>
+    <t>Investigacion Figma</t>
+  </si>
+  <si>
+    <t>API Twitter</t>
+  </si>
+  <si>
+    <t>La API que utilizamos para la creacion del dataset de entrenamiento  anuncio que dejara de ser gratuita en una semana, por lo que extendimos la extraccion de datos para obtener data aplicable a la cuarta etapa (clasificador de texto) ahora que podemos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reunion muestra de prototipo </t>
+  </si>
+  <si>
+    <t>Nos reunimos con lucia, bruno y martin para hacer la muestra del prototipo creado y registrar los cambios necesarios.</t>
+  </si>
+  <si>
+    <t>Runion con bruno: determinacion de entidades a etiquetar, pruebas con label studio, charla de creacion de dataset y entrenamientos.</t>
+  </si>
+  <si>
+    <t>Reunion Bruno</t>
   </si>
 </sst>
 </file>
@@ -202,7 +244,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,12 +277,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -378,11 +438,258 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -420,34 +727,125 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -760,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,18 +1252,78 @@
         <v>44909</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="11" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>44912</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>44917</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>44933</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>44959</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>44960</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>44963</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="17" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -923,7 +1381,7 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="17">
+      <c r="B3" s="37">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -932,40 +1390,40 @@
       <c r="D3" s="12">
         <v>44858</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="41">
         <v>44914</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="45">
         <v>160</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="12">
         <v>44879</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="17"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="12">
         <v>44900</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
     </row>
     <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="18">
+      <c r="B6" s="38">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -974,52 +1432,52 @@
       <c r="D6" s="12">
         <v>44914</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="42">
         <v>44991</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="45">
         <v>220</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="45"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="12">
         <v>44942</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="12">
         <v>44970</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
     </row>
     <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="12">
         <v>44984</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
     </row>
     <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="19">
+      <c r="B10" s="39">
         <v>3</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1028,52 +1486,52 @@
       <c r="D10" s="12">
         <v>44991</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="43">
         <v>45068</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="45">
         <v>220</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="45"/>
     </row>
     <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="12">
         <v>45019</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
     </row>
     <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="12">
         <v>45047</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
     </row>
     <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="19"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="12">
         <v>45061</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="20">
+      <c r="B14" s="40">
         <v>4</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1082,40 +1540,48 @@
       <c r="D14" s="12">
         <v>45068</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="44">
         <v>44773</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="45">
         <v>200</v>
       </c>
-      <c r="G14" s="16"/>
+      <c r="G14" s="45"/>
     </row>
     <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="12">
         <v>45089</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="20"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="12">
         <v>45103</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="G14:G16"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
@@ -1124,14 +1590,6 @@
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="E10:E13"/>
     <mergeCell ref="E14:E16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="G14:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1140,23 +1598,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G17"/>
+  <dimension ref="B1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="57.42578125" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" customWidth="1"/>
+    <col min="5" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1169,15 +1627,18 @@
       <c r="E2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="17">
+      <c r="H2" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="49">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -1186,215 +1647,252 @@
       <c r="D3" s="12">
         <v>44858</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="54">
         <v>44914</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="19"/>
+      <c r="G3" s="45">
         <v>160</v>
       </c>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
+      <c r="H3" s="45">
+        <f>40+34</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="50"/>
       <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="12">
         <v>44879</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="17"/>
-      <c r="C5" s="8" t="s">
+      <c r="E4" s="55"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="51"/>
+      <c r="C5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="24">
         <v>44900</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="17"/>
-      <c r="C6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="18">
+      <c r="E5" s="55"/>
+      <c r="F5" s="27">
+        <v>44912</v>
+      </c>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="52">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C6" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="45"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="53"/>
+      <c r="C7" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36">
+        <v>44942</v>
+      </c>
+      <c r="G7" s="46"/>
+      <c r="H7" s="45"/>
+    </row>
+    <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="38">
+        <v>3</v>
+      </c>
+      <c r="C8" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D8" s="26">
         <v>44914</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E8" s="47">
+        <v>44990</v>
+      </c>
+      <c r="F8" s="28"/>
+      <c r="G8" s="45">
+        <v>220</v>
+      </c>
+      <c r="H8" s="48"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="38"/>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="12">
+        <v>44942</v>
+      </c>
+      <c r="E9" s="38"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="48"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="38"/>
+      <c r="C10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="12">
+        <v>44970</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="48"/>
+    </row>
+    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="38"/>
+      <c r="C11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="12">
+        <v>44984</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="48"/>
+    </row>
+    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="39">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="12">
         <v>44991</v>
       </c>
-      <c r="F7" s="16">
+      <c r="E12" s="43">
+        <v>45068</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="45">
         <v>220</v>
       </c>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="12">
-        <v>44942</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
-      <c r="C9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="12">
-        <v>44970</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18"/>
-      <c r="C10" s="9" t="s">
+      <c r="H12" s="45"/>
+    </row>
+    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="39"/>
+      <c r="C13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="12">
+        <v>45019</v>
+      </c>
+      <c r="E13" s="39"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+    </row>
+    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="39"/>
+      <c r="C14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="12">
+        <v>45047</v>
+      </c>
+      <c r="E14" s="39"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="39"/>
+      <c r="C15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="12">
-        <v>44984</v>
-      </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="19">
-        <v>3</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="12">
-        <v>44991</v>
-      </c>
-      <c r="E11" s="23">
+      <c r="D15" s="12">
+        <v>45061</v>
+      </c>
+      <c r="E15" s="39"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="40">
+        <v>5</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="12">
         <v>45068</v>
       </c>
-      <c r="F11" s="16">
-        <v>220</v>
-      </c>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="12">
-        <v>45019</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-      <c r="C13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="12">
-        <v>45047</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="19"/>
-      <c r="C14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="12">
-        <v>45061</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="20">
-        <v>4</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="12">
-        <v>45068</v>
-      </c>
-      <c r="E15" s="24">
+      <c r="E16" s="44">
         <v>44773</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F16" s="21"/>
+      <c r="G16" s="45">
         <v>200</v>
       </c>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
-      <c r="C16" s="7" t="s">
+      <c r="H16" s="45"/>
+    </row>
+    <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="40"/>
+      <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D17" s="12">
         <v>45089</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="20"/>
-      <c r="C17" s="8" t="s">
+      <c r="E17" s="40"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="40"/>
+      <c r="C18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D18" s="12">
         <v>45103</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G15:G17"/>
+  <mergeCells count="17">
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="G3:G7"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="E3:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add: filtro para mostrar solo entidades de cierto tipo
</commit_message>
<xml_diff>
--- a/Minutas.xlsx
+++ b/Minutas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
   <si>
     <t>Fecha</t>
   </si>
@@ -275,6 +275,18 @@
   </si>
   <si>
     <t>Nos reunimos con bruno.</t>
+  </si>
+  <si>
+    <t>Estas no me acuerdo del dia a mediados de noviembre</t>
+  </si>
+  <si>
+    <t>Columna1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reunion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nos reunimos con bruno, lucia , martin y santiago trigo para hablar de la interfaz, presentacion de la informacion y ultimos cambios </t>
   </si>
 </sst>
 </file>
@@ -872,31 +884,31 @@
     <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -963,12 +975,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:D43" totalsRowShown="0">
-  <autoFilter ref="B3:D43"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:E43" totalsRowShown="0">
+  <autoFilter ref="B3:E43"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Fecha" dataDxfId="2"/>
     <tableColumn id="2" name="Evento" dataDxfId="1"/>
     <tableColumn id="3" name="Descripcion" dataDxfId="0"/>
+    <tableColumn id="4" name="Columna1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1237,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H29"/>
+  <dimension ref="B3:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G36" sqref="G34:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,6 +1273,9 @@
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="4" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -1542,6 +1558,45 @@
       </c>
       <c r="C29" s="2" t="s">
         <v>75</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>45231</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>45231</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>45261</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1590,7 +1645,7 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="39">
+      <c r="B3" s="38">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -1599,40 +1654,40 @@
       <c r="D3" s="12">
         <v>44858</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="42">
         <v>44914</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="46">
         <v>160</v>
       </c>
-      <c r="G3" s="38"/>
+      <c r="G3" s="46"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="12">
         <v>44879</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="39"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="12">
         <v>44900</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
     </row>
     <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="40">
+      <c r="B6" s="39">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1641,52 +1696,52 @@
       <c r="D6" s="12">
         <v>44914</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="43">
         <v>44991</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="46">
         <v>220</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="46"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="12">
         <v>44942</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="12">
         <v>44970</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
     </row>
     <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="40"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="12">
         <v>44984</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
     </row>
     <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="41">
+      <c r="B10" s="40">
         <v>3</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1695,52 +1750,52 @@
       <c r="D10" s="12">
         <v>44991</v>
       </c>
-      <c r="E10" s="45">
+      <c r="E10" s="44">
         <v>45068</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="46">
         <v>220</v>
       </c>
-      <c r="G10" s="38"/>
+      <c r="G10" s="46"/>
     </row>
     <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="12">
         <v>45019</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
     </row>
     <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="12">
         <v>45047</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
     </row>
     <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="41"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="12">
         <v>45061</v>
       </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="42">
+      <c r="B14" s="41">
         <v>4</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1749,40 +1804,48 @@
       <c r="D14" s="12">
         <v>45068</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <v>44773</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="46">
         <v>200</v>
       </c>
-      <c r="G14" s="38"/>
+      <c r="G14" s="46"/>
     </row>
     <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="12">
         <v>45089</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="42"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="12">
         <v>45103</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="G14:G16"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
@@ -1791,14 +1854,6 @@
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="E10:E13"/>
     <mergeCell ref="E14:E16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="G14:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1860,10 +1915,10 @@
         <v>44914</v>
       </c>
       <c r="F3" s="19"/>
-      <c r="G3" s="38">
+      <c r="G3" s="46">
         <v>160</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="46">
         <f>40+34</f>
         <v>74</v>
       </c>
@@ -1878,8 +1933,8 @@
       </c>
       <c r="E4" s="56"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="52"/>
@@ -1893,8 +1948,8 @@
       <c r="F5" s="27">
         <v>44912</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="53">
@@ -1907,7 +1962,7 @@
       <c r="E6" s="31"/>
       <c r="F6" s="32"/>
       <c r="G6" s="47"/>
-      <c r="H6" s="38"/>
+      <c r="H6" s="46"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="54"/>
@@ -1920,10 +1975,10 @@
         <v>44942</v>
       </c>
       <c r="G7" s="47"/>
-      <c r="H7" s="38"/>
+      <c r="H7" s="46"/>
     </row>
     <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="40">
+      <c r="B8" s="39">
         <v>3</v>
       </c>
       <c r="C8" s="25" t="s">
@@ -1936,7 +1991,7 @@
         <v>44991</v>
       </c>
       <c r="F8" s="28"/>
-      <c r="G8" s="38">
+      <c r="G8" s="46">
         <v>220</v>
       </c>
       <c r="H8" s="49">
@@ -1945,51 +2000,51 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="12">
         <v>44942</v>
       </c>
-      <c r="E9" s="40"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="38"/>
+      <c r="G9" s="46"/>
       <c r="H9" s="49"/>
       <c r="I9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="12">
         <v>44970</v>
       </c>
-      <c r="E10" s="40"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="38"/>
+      <c r="G10" s="46"/>
       <c r="H10" s="49"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="40"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="12">
         <v>44984</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="37">
         <v>45032</v>
       </c>
-      <c r="G11" s="38"/>
+      <c r="G11" s="46"/>
       <c r="H11" s="49"/>
     </row>
     <row r="12" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="41">
+      <c r="B12" s="40">
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1998,56 +2053,56 @@
       <c r="D12" s="12">
         <v>44991</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="44">
         <v>45068</v>
       </c>
       <c r="F12" s="20"/>
-      <c r="G12" s="38">
+      <c r="G12" s="46">
         <v>220</v>
       </c>
-      <c r="H12" s="38"/>
+      <c r="H12" s="46"/>
     </row>
     <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="12">
         <v>45019</v>
       </c>
-      <c r="E13" s="41"/>
+      <c r="E13" s="40"/>
       <c r="F13" s="17"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
     </row>
     <row r="14" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="12">
         <v>45047</v>
       </c>
-      <c r="E14" s="41"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="41"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="12">
         <v>45061</v>
       </c>
-      <c r="E15" s="41"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="42">
+      <c r="B16" s="41">
         <v>5</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -2056,43 +2111,51 @@
       <c r="D16" s="12">
         <v>45068</v>
       </c>
-      <c r="E16" s="46">
+      <c r="E16" s="45">
         <v>44773</v>
       </c>
       <c r="F16" s="21"/>
-      <c r="G16" s="38">
+      <c r="G16" s="46">
         <v>200</v>
       </c>
-      <c r="H16" s="38"/>
+      <c r="H16" s="46"/>
     </row>
     <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="42"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="12">
         <v>45089</v>
       </c>
-      <c r="E17" s="42"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="42"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="12">
         <v>45103</v>
       </c>
-      <c r="E18" s="42"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="18"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="H16:H18"/>
     <mergeCell ref="G3:G7"/>
     <mergeCell ref="H3:H7"/>
     <mergeCell ref="B8:B11"/>
@@ -2102,14 +2165,6 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="E3:E5"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="H16:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>